<commit_message>
Added aanmelding and intake form to datadump
</commit_message>
<xml_diff>
--- a/Ordina.StichtingNuTwente/Ordina.StichtingNuTwente.WebApp/DataDumpTemplate.xlsx
+++ b/Ordina.StichtingNuTwente/Ordina.StichtingNuTwente.WebApp/DataDumpTemplate.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkl32015\source\repos\Stichting-NUTwente\Ordina.StichtingNuTwente\Ordina.StichtingNuTwente.WebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92486ACF-6A92-49DA-9E97-1CD147EF378B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A031126-F6C1-41EB-81C8-517B618E354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastgezinnen" sheetId="1" r:id="rId1"/>
+    <sheet name="AanmeldFormulier" sheetId="2" r:id="rId2"/>
+    <sheet name="IntakeFormulier" sheetId="3" r:id="rId3"/>
+    <sheet name="Plaatsingen" sheetId="4" r:id="rId4"/>
+    <sheet name="Vrijwilligers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -382,7 +386,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C685993-2301-40F2-9702-3294D1BBFEAA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB32687-578A-44E9-8070-3CF7471F6221}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1B163B-A2F6-4AC0-92C7-2FF86528D732}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA2A36E-7EAA-4D49-A631-BB14FEEFA457}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C0FDD2-C1A8-4BBB-9FCF-544FD2F71E79}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added more data dumps
</commit_message>
<xml_diff>
--- a/Ordina.StichtingNuTwente/Ordina.StichtingNuTwente.WebApp/DataDumpTemplate.xlsx
+++ b/Ordina.StichtingNuTwente/Ordina.StichtingNuTwente.WebApp/DataDumpTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkl32015\source\repos\Stichting-NUTwente\Ordina.StichtingNuTwente\Ordina.StichtingNuTwente.WebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A031126-F6C1-41EB-81C8-517B618E354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C303CB1B-017B-47D9-A036-3051B57611AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastgezinnen" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="IntakeFormulier" sheetId="3" r:id="rId3"/>
     <sheet name="Plaatsingen" sheetId="4" r:id="rId4"/>
     <sheet name="Vrijwilligers" sheetId="5" r:id="rId5"/>
+    <sheet name="ContactLogs" sheetId="6" r:id="rId6"/>
+    <sheet name="Comments" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -398,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB32687-578A-44E9-8070-3CF7471F6221}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -442,4 +444,28 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFA765A-04DF-43A9-8780-86FDFB68E313}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE56B33-4873-4BC9-95CE-27E0C701AB61}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>